<commit_message>
foutje in pinmapping aangepast
</commit_message>
<xml_diff>
--- a/programmingdocumentation/pinmapping_SCGC5values.xlsx
+++ b/programmingdocumentation/pinmapping_SCGC5values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BBC200-8661-4E17-8B04-D00CE8B02FBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5890FD-984B-425E-9DD8-A15BCD390F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2741910F-6369-4123-A32C-77151700AA90}"/>
+    <workbookView xWindow="768" yWindow="456" windowWidth="17280" windowHeight="9420" xr2:uid="{2741910F-6369-4123-A32C-77151700AA90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>led AP</t>
   </si>
@@ -159,6 +159,63 @@
   </si>
   <si>
     <t>PTE26</t>
+  </si>
+  <si>
+    <t>lcd</t>
+  </si>
+  <si>
+    <t>nCS</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>A0(miso?)</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>mosi</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>PTD0</t>
+  </si>
+  <si>
+    <t>PTC3</t>
+  </si>
+  <si>
+    <t>PTD1</t>
+  </si>
+  <si>
+    <t>PTD3</t>
+  </si>
+  <si>
+    <t>PTD2</t>
+  </si>
+  <si>
+    <t>speaker</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>PTC2</t>
   </si>
 </sst>
 </file>
@@ -537,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090F3B29-FDBE-471A-B15A-436A497A39A2}">
-  <dimension ref="A2:I17"/>
+  <dimension ref="A2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +606,7 @@
     <col min="7" max="7" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -567,7 +624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -584,7 +641,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -592,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>3</v>
@@ -601,7 +658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -609,7 +666,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>17</v>
@@ -618,7 +675,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
@@ -626,7 +683,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -642,7 +699,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -650,7 +707,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -658,7 +715,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -666,12 +723,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -683,7 +735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
@@ -694,7 +746,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
@@ -705,7 +757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
@@ -716,7 +768,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
@@ -727,7 +779,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
@@ -736,6 +788,96 @@
       </c>
       <c r="D17" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>